<commit_message>
Updated the file old date referances.
</commit_message>
<xml_diff>
--- a/docs/unit1/0_getting_started/(Starter-Workbook)-HW-A-Tour-of-Class-Resources.xlsx
+++ b/docs/unit1/0_getting_started/(Starter-Workbook)-HW-A-Tour-of-Class-Resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fs-caedm\homes\.caedm\My Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandanwilliamson/Desktop/CCE 270/content/docs/unit1/0_getting_started/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C61873-7456-41C4-BD87-27058D7390E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53855E2-9C6C-6E42-8879-B61DC57FE767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{935E1006-0B13-48A8-B071-906A587FBB91}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="21660" activeTab="1" xr2:uid="{935E1006-0B13-48A8-B071-906A587FBB91}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>3. What are the next 5 things due for this class?</t>
   </si>
   <si>
-    <t>3. On our Class Website, navigate to the "Office Hours" tab and take a screenshot of the office hours for September 8th to September 12th.</t>
-  </si>
-  <si>
     <t>4. Post a message in Microsoft Teams in the Homework Help channel. Take a screenshot.</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>2. Take a picture of your OneDrive folder with your HW starter sheet in it. Make sure the screenshot shows the folder name you created in Part 1.</t>
+  </si>
+  <si>
+    <t>3. On our Class Website, navigate to the "Office Hours" tab and take a screenshot of the office hours for the first full week of the semester.</t>
   </si>
 </sst>
 </file>
@@ -117,9 +117,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -157,7 +157,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -263,7 +263,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -405,7 +405,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -419,32 +419,32 @@
       <selection activeCell="B3" sqref="B1:OI1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="127.7109375" customWidth="1"/>
+    <col min="1" max="1" width="127.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -460,38 +460,38 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="127.7109375" customWidth="1"/>
+    <col min="1" max="1" width="127.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="240" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="240" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" ht="240" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="240" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" ht="240" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="240" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="240" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:1" ht="240" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>